<commit_message>
Update up to 2023-02-10
</commit_message>
<xml_diff>
--- a/nifty 100.xlsx
+++ b/nifty 100.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2999"/>
+  <dimension ref="A1:E3004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51423,6 +51423,91 @@
         <v>1.44</v>
       </c>
     </row>
+    <row r="3000">
+      <c r="A3000" s="4" t="n">
+        <v>44963</v>
+      </c>
+      <c r="B3000" t="n">
+        <v>23451.89</v>
+      </c>
+      <c r="C3000" t="n">
+        <v>21.46</v>
+      </c>
+      <c r="D3000" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="E3000" t="n">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="3001">
+      <c r="A3001" s="4" t="n">
+        <v>44964</v>
+      </c>
+      <c r="B3001" t="n">
+        <v>23396.47</v>
+      </c>
+      <c r="C3001" t="n">
+        <v>21.19</v>
+      </c>
+      <c r="D3001" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="E3001" t="n">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="3002">
+      <c r="A3002" s="4" t="n">
+        <v>44965</v>
+      </c>
+      <c r="B3002" t="n">
+        <v>23598.72</v>
+      </c>
+      <c r="C3002" t="n">
+        <v>21.77</v>
+      </c>
+      <c r="D3002" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="E3002" t="n">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="3003">
+      <c r="A3003" s="4" t="n">
+        <v>44966</v>
+      </c>
+      <c r="B3003" t="n">
+        <v>23604.05</v>
+      </c>
+      <c r="C3003" t="n">
+        <v>21.75</v>
+      </c>
+      <c r="D3003" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="E3003" t="n">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="3004">
+      <c r="A3004" s="4" t="n">
+        <v>44967</v>
+      </c>
+      <c r="B3004" t="n">
+        <v>23553.54</v>
+      </c>
+      <c r="C3004" t="n">
+        <v>21.71</v>
+      </c>
+      <c r="D3004" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="E3004" t="n">
+        <v>1.45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update up to 2025-01-14
</commit_message>
<xml_diff>
--- a/nifty 100.xlsx
+++ b/nifty 100.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3407"/>
+  <dimension ref="A1:E3480"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -58361,6 +58361,1247 @@
         <v>1.14</v>
       </c>
     </row>
+    <row r="3408">
+      <c r="A3408" s="5" t="n">
+        <v>45565</v>
+      </c>
+      <c r="B3408" t="n">
+        <v>36486.84</v>
+      </c>
+      <c r="C3408" t="n">
+        <v>24.88</v>
+      </c>
+      <c r="D3408" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="E3408" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="3409">
+      <c r="A3409" s="5" t="n">
+        <v>45566</v>
+      </c>
+      <c r="B3409" t="n">
+        <v>36480.21</v>
+      </c>
+      <c r="C3409" t="n">
+        <v>24.87</v>
+      </c>
+      <c r="D3409" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="E3409" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="3410">
+      <c r="A3410" s="5" t="n">
+        <v>45568</v>
+      </c>
+      <c r="B3410" t="n">
+        <v>35693.21</v>
+      </c>
+      <c r="C3410" t="n">
+        <v>24.34</v>
+      </c>
+      <c r="D3410" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="E3410" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="3411">
+      <c r="A3411" s="5" t="n">
+        <v>45569</v>
+      </c>
+      <c r="B3411" t="n">
+        <v>35354.99</v>
+      </c>
+      <c r="C3411" t="n">
+        <v>24.11</v>
+      </c>
+      <c r="D3411" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E3411" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3412">
+      <c r="A3412" s="5" t="n">
+        <v>45572</v>
+      </c>
+      <c r="B3412" t="n">
+        <v>34939.32</v>
+      </c>
+      <c r="C3412" t="n">
+        <v>23.82</v>
+      </c>
+      <c r="D3412" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="E3412" t="n">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3413">
+      <c r="A3413" s="5" t="n">
+        <v>45573</v>
+      </c>
+      <c r="B3413" t="n">
+        <v>35356.84</v>
+      </c>
+      <c r="C3413" t="n">
+        <v>24.11</v>
+      </c>
+      <c r="D3413" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E3413" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3414">
+      <c r="A3414" s="5" t="n">
+        <v>45574</v>
+      </c>
+      <c r="B3414" t="n">
+        <v>35382.94</v>
+      </c>
+      <c r="C3414" t="n">
+        <v>24.12</v>
+      </c>
+      <c r="D3414" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E3414" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3415">
+      <c r="A3415" s="5" t="n">
+        <v>45575</v>
+      </c>
+      <c r="B3415" t="n">
+        <v>35386.82</v>
+      </c>
+      <c r="C3415" t="n">
+        <v>24.13</v>
+      </c>
+      <c r="D3415" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E3415" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3416">
+      <c r="A3416" s="5" t="n">
+        <v>45576</v>
+      </c>
+      <c r="B3416" t="n">
+        <v>35352.41</v>
+      </c>
+      <c r="C3416" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="D3416" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E3416" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3417">
+      <c r="A3417" s="5" t="n">
+        <v>45579</v>
+      </c>
+      <c r="B3417" t="n">
+        <v>35547.57</v>
+      </c>
+      <c r="C3417" t="n">
+        <v>24.24</v>
+      </c>
+      <c r="D3417" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="E3417" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3418">
+      <c r="A3418" s="5" t="n">
+        <v>45580</v>
+      </c>
+      <c r="B3418" t="n">
+        <v>35481.33</v>
+      </c>
+      <c r="C3418" t="n">
+        <v>24.18</v>
+      </c>
+      <c r="D3418" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="E3418" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3419">
+      <c r="A3419" s="5" t="n">
+        <v>45581</v>
+      </c>
+      <c r="B3419" t="n">
+        <v>35357.84</v>
+      </c>
+      <c r="C3419" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="D3419" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E3419" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3420">
+      <c r="A3420" s="5" t="n">
+        <v>45582</v>
+      </c>
+      <c r="B3420" t="n">
+        <v>34960.64</v>
+      </c>
+      <c r="C3420" t="n">
+        <v>23.83</v>
+      </c>
+      <c r="D3420" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="E3420" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3421">
+      <c r="A3421" s="5" t="n">
+        <v>45583</v>
+      </c>
+      <c r="B3421" t="n">
+        <v>35083.28</v>
+      </c>
+      <c r="C3421" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="D3421" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E3421" t="n">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3422">
+      <c r="A3422" s="5" t="n">
+        <v>45586</v>
+      </c>
+      <c r="B3422" t="n">
+        <v>34928.13</v>
+      </c>
+      <c r="C3422" t="n">
+        <v>23.75</v>
+      </c>
+      <c r="D3422" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="E3422" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3423">
+      <c r="A3423" s="5" t="n">
+        <v>45587</v>
+      </c>
+      <c r="B3423" t="n">
+        <v>34400.21</v>
+      </c>
+      <c r="C3423" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="D3423" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E3423" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3424">
+      <c r="A3424" s="5" t="n">
+        <v>45588</v>
+      </c>
+      <c r="B3424" t="n">
+        <v>34362.99</v>
+      </c>
+      <c r="C3424" t="n">
+        <v>23.27</v>
+      </c>
+      <c r="D3424" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E3424" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3425">
+      <c r="A3425" s="5" t="n">
+        <v>45589</v>
+      </c>
+      <c r="B3425" t="n">
+        <v>34301.75</v>
+      </c>
+      <c r="C3425" t="n">
+        <v>23.21</v>
+      </c>
+      <c r="D3425" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="E3425" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3426">
+      <c r="A3426" s="5" t="n">
+        <v>45590</v>
+      </c>
+      <c r="B3426" t="n">
+        <v>33958.49</v>
+      </c>
+      <c r="C3426" t="n">
+        <v>22.97</v>
+      </c>
+      <c r="D3426" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="E3426" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3427">
+      <c r="A3427" s="5" t="n">
+        <v>45593</v>
+      </c>
+      <c r="B3427" t="n">
+        <v>34166.46</v>
+      </c>
+      <c r="C3427" t="n">
+        <v>23.14</v>
+      </c>
+      <c r="D3427" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="E3427" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="3428">
+      <c r="A3428" s="5" t="n">
+        <v>45594</v>
+      </c>
+      <c r="B3428" t="n">
+        <v>34384.01</v>
+      </c>
+      <c r="C3428" t="n">
+        <v>23.41</v>
+      </c>
+      <c r="D3428" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E3428" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3429">
+      <c r="A3429" s="5" t="n">
+        <v>45595</v>
+      </c>
+      <c r="B3429" t="n">
+        <v>34212.58</v>
+      </c>
+      <c r="C3429" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="D3429" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="E3429" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3430">
+      <c r="A3430" s="5" t="n">
+        <v>45596</v>
+      </c>
+      <c r="B3430" t="n">
+        <v>34034.49</v>
+      </c>
+      <c r="C3430" t="n">
+        <v>23.14</v>
+      </c>
+      <c r="D3430" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="E3430" t="n">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="3431">
+      <c r="A3431" s="5" t="n">
+        <v>45597</v>
+      </c>
+      <c r="B3431" t="n">
+        <v>34204.39</v>
+      </c>
+      <c r="C3431" t="n">
+        <v>23.26</v>
+      </c>
+      <c r="D3431" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="E3431" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3432">
+      <c r="A3432" s="5" t="n">
+        <v>45600</v>
+      </c>
+      <c r="B3432" t="n">
+        <v>33760.47</v>
+      </c>
+      <c r="C3432" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="D3432" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="E3432" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3433">
+      <c r="A3433" s="5" t="n">
+        <v>45601</v>
+      </c>
+      <c r="B3433" t="n">
+        <v>34036.2</v>
+      </c>
+      <c r="C3433" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="D3433" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="E3433" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3434">
+      <c r="A3434" s="5" t="n">
+        <v>45602</v>
+      </c>
+      <c r="B3434" t="n">
+        <v>34507.77</v>
+      </c>
+      <c r="C3434" t="n">
+        <v>23.42</v>
+      </c>
+      <c r="D3434" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="E3434" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3435">
+      <c r="A3435" s="5" t="n">
+        <v>45603</v>
+      </c>
+      <c r="B3435" t="n">
+        <v>34112.08</v>
+      </c>
+      <c r="C3435" t="n">
+        <v>23.15</v>
+      </c>
+      <c r="D3435" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="E3435" t="n">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="3436">
+      <c r="A3436" s="5" t="n">
+        <v>45604</v>
+      </c>
+      <c r="B3436" t="n">
+        <v>33967.44</v>
+      </c>
+      <c r="C3436" t="n">
+        <v>22.87</v>
+      </c>
+      <c r="D3436" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="E3436" t="n">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="3437">
+      <c r="A3437" s="5" t="n">
+        <v>45607</v>
+      </c>
+      <c r="B3437" t="n">
+        <v>33981.48</v>
+      </c>
+      <c r="C3437" t="n">
+        <v>22.86</v>
+      </c>
+      <c r="D3437" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="E3437" t="n">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="3438">
+      <c r="A3438" s="5" t="n">
+        <v>45608</v>
+      </c>
+      <c r="B3438" t="n">
+        <v>33577.34</v>
+      </c>
+      <c r="C3438" t="n">
+        <v>22.41</v>
+      </c>
+      <c r="D3438" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="E3438" t="n">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="3439">
+      <c r="A3439" s="5" t="n">
+        <v>45609</v>
+      </c>
+      <c r="B3439" t="n">
+        <v>33076.62</v>
+      </c>
+      <c r="C3439" t="n">
+        <v>22.12</v>
+      </c>
+      <c r="D3439" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E3439" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="3440">
+      <c r="A3440" s="5" t="n">
+        <v>45610</v>
+      </c>
+      <c r="B3440" t="n">
+        <v>33108.05</v>
+      </c>
+      <c r="C3440" t="n">
+        <v>22.13</v>
+      </c>
+      <c r="D3440" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E3440" t="n">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="3441">
+      <c r="A3441" s="5" t="n">
+        <v>45614</v>
+      </c>
+      <c r="B3441" t="n">
+        <v>33019.66</v>
+      </c>
+      <c r="C3441" t="n">
+        <v>22.06</v>
+      </c>
+      <c r="D3441" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="E3441" t="n">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="3442">
+      <c r="A3442" s="5" t="n">
+        <v>45615</v>
+      </c>
+      <c r="B3442" t="n">
+        <v>33120.54</v>
+      </c>
+      <c r="C3442" t="n">
+        <v>22.14</v>
+      </c>
+      <c r="D3442" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E3442" t="n">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="3443">
+      <c r="A3443" s="5" t="n">
+        <v>45617</v>
+      </c>
+      <c r="B3443" t="n">
+        <v>32794.98</v>
+      </c>
+      <c r="C3443" t="n">
+        <v>21.92</v>
+      </c>
+      <c r="D3443" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="E3443" t="n">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="3444">
+      <c r="A3444" s="5" t="n">
+        <v>45618</v>
+      </c>
+      <c r="B3444" t="n">
+        <v>33501.86</v>
+      </c>
+      <c r="C3444" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="D3444" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="E3444" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3445">
+      <c r="A3445" s="5" t="n">
+        <v>45621</v>
+      </c>
+      <c r="B3445" t="n">
+        <v>33962.87</v>
+      </c>
+      <c r="C3445" t="n">
+        <v>22.7</v>
+      </c>
+      <c r="D3445" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="E3445" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3446">
+      <c r="A3446" s="5" t="n">
+        <v>45622</v>
+      </c>
+      <c r="B3446" t="n">
+        <v>33948.51</v>
+      </c>
+      <c r="C3446" t="n">
+        <v>22.69</v>
+      </c>
+      <c r="D3446" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="E3446" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3447">
+      <c r="A3447" s="5" t="n">
+        <v>45623</v>
+      </c>
+      <c r="B3447" t="n">
+        <v>34127.93</v>
+      </c>
+      <c r="C3447" t="n">
+        <v>22.81</v>
+      </c>
+      <c r="D3447" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="E3447" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3448">
+      <c r="A3448" s="5" t="n">
+        <v>45624</v>
+      </c>
+      <c r="B3448" t="n">
+        <v>33749</v>
+      </c>
+      <c r="C3448" t="n">
+        <v>22.56</v>
+      </c>
+      <c r="D3448" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="E3448" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3449">
+      <c r="A3449" s="5" t="n">
+        <v>45625</v>
+      </c>
+      <c r="B3449" t="n">
+        <v>34044.81</v>
+      </c>
+      <c r="C3449" t="n">
+        <v>22.76</v>
+      </c>
+      <c r="D3449" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="E3449" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3450">
+      <c r="A3450" s="5" t="n">
+        <v>45628</v>
+      </c>
+      <c r="B3450" t="n">
+        <v>34240.75</v>
+      </c>
+      <c r="C3450" t="n">
+        <v>22.89</v>
+      </c>
+      <c r="D3450" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="E3450" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3451">
+      <c r="A3451" s="5" t="n">
+        <v>45629</v>
+      </c>
+      <c r="B3451" t="n">
+        <v>34505.83</v>
+      </c>
+      <c r="C3451" t="n">
+        <v>23.06</v>
+      </c>
+      <c r="D3451" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="E3451" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3452">
+      <c r="A3452" s="5" t="n">
+        <v>45630</v>
+      </c>
+      <c r="B3452" t="n">
+        <v>34553.64</v>
+      </c>
+      <c r="C3452" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="D3452" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E3452" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="3453">
+      <c r="A3453" s="5" t="n">
+        <v>45631</v>
+      </c>
+      <c r="B3453" t="n">
+        <v>34865.41</v>
+      </c>
+      <c r="C3453" t="n">
+        <v>23.31</v>
+      </c>
+      <c r="D3453" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E3453" t="n">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3454">
+      <c r="A3454" s="5" t="n">
+        <v>45632</v>
+      </c>
+      <c r="B3454" t="n">
+        <v>34873.66</v>
+      </c>
+      <c r="C3454" t="n">
+        <v>23.31</v>
+      </c>
+      <c r="D3454" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E3454" t="n">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3455">
+      <c r="A3455" s="5" t="n">
+        <v>45635</v>
+      </c>
+      <c r="B3455" t="n">
+        <v>34778.95</v>
+      </c>
+      <c r="C3455" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="D3455" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="E3455" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="3456">
+      <c r="A3456" s="5" t="n">
+        <v>45636</v>
+      </c>
+      <c r="B3456" t="n">
+        <v>34787.08</v>
+      </c>
+      <c r="C3456" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="D3456" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="E3456" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="3457">
+      <c r="A3457" s="5" t="n">
+        <v>45637</v>
+      </c>
+      <c r="B3457" t="n">
+        <v>34834.43</v>
+      </c>
+      <c r="C3457" t="n">
+        <v>23.28</v>
+      </c>
+      <c r="D3457" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E3457" t="n">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3458">
+      <c r="A3458" s="5" t="n">
+        <v>45638</v>
+      </c>
+      <c r="B3458" t="n">
+        <v>34713.96</v>
+      </c>
+      <c r="C3458" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="D3458" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="E3458" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3459">
+      <c r="A3459" s="5" t="n">
+        <v>45639</v>
+      </c>
+      <c r="B3459" t="n">
+        <v>34956.09</v>
+      </c>
+      <c r="C3459" t="n">
+        <v>23.37</v>
+      </c>
+      <c r="D3459" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="E3459" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3460">
+      <c r="A3460" s="5" t="n">
+        <v>45642</v>
+      </c>
+      <c r="B3460" t="n">
+        <v>34858.65</v>
+      </c>
+      <c r="C3460" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="D3460" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E3460" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3461">
+      <c r="A3461" s="5" t="n">
+        <v>45643</v>
+      </c>
+      <c r="B3461" t="n">
+        <v>34408.57</v>
+      </c>
+      <c r="C3461" t="n">
+        <v>23</v>
+      </c>
+      <c r="D3461" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="E3461" t="n">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3462">
+      <c r="A3462" s="5" t="n">
+        <v>45644</v>
+      </c>
+      <c r="B3462" t="n">
+        <v>34158.48</v>
+      </c>
+      <c r="C3462" t="n">
+        <v>22.83</v>
+      </c>
+      <c r="D3462" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="E3462" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="3463">
+      <c r="A3463" s="5" t="n">
+        <v>45645</v>
+      </c>
+      <c r="B3463" t="n">
+        <v>33815.14</v>
+      </c>
+      <c r="C3463" t="n">
+        <v>22.6</v>
+      </c>
+      <c r="D3463" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="E3463" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3464">
+      <c r="A3464" s="5" t="n">
+        <v>45646</v>
+      </c>
+      <c r="B3464" t="n">
+        <v>33222.58</v>
+      </c>
+      <c r="C3464" t="n">
+        <v>22.21</v>
+      </c>
+      <c r="D3464" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E3464" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3465">
+      <c r="A3465" s="5" t="n">
+        <v>45649</v>
+      </c>
+      <c r="B3465" t="n">
+        <v>33427.62</v>
+      </c>
+      <c r="C3465" t="n">
+        <v>22.34</v>
+      </c>
+      <c r="D3465" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="E3465" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3466">
+      <c r="A3466" s="5" t="n">
+        <v>45650</v>
+      </c>
+      <c r="B3466" t="n">
+        <v>33394.26</v>
+      </c>
+      <c r="C3466" t="n">
+        <v>22.32</v>
+      </c>
+      <c r="D3466" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="E3466" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3467">
+      <c r="A3467" s="5" t="n">
+        <v>45652</v>
+      </c>
+      <c r="B3467" t="n">
+        <v>33447.03</v>
+      </c>
+      <c r="C3467" t="n">
+        <v>22.35</v>
+      </c>
+      <c r="D3467" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="E3467" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3468">
+      <c r="A3468" s="5" t="n">
+        <v>45653</v>
+      </c>
+      <c r="B3468" t="n">
+        <v>33475.1</v>
+      </c>
+      <c r="C3468" t="n">
+        <v>22.37</v>
+      </c>
+      <c r="D3468" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="E3468" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3469">
+      <c r="A3469" s="5" t="n">
+        <v>45656</v>
+      </c>
+      <c r="B3469" t="n">
+        <v>33296.75</v>
+      </c>
+      <c r="C3469" t="n">
+        <v>22.25</v>
+      </c>
+      <c r="D3469" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E3469" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3470">
+      <c r="A3470" s="5" t="n">
+        <v>45657</v>
+      </c>
+      <c r="B3470" t="n">
+        <v>33289.71</v>
+      </c>
+      <c r="C3470" t="n">
+        <v>22.31</v>
+      </c>
+      <c r="D3470" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="E3470" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3471">
+      <c r="A3471" s="5" t="n">
+        <v>45658</v>
+      </c>
+      <c r="B3471" t="n">
+        <v>33425.78</v>
+      </c>
+      <c r="C3471" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="D3471" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="E3471" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3472">
+      <c r="A3472" s="5" t="n">
+        <v>45659</v>
+      </c>
+      <c r="B3472" t="n">
+        <v>34014.41</v>
+      </c>
+      <c r="C3472" t="n">
+        <v>22.79</v>
+      </c>
+      <c r="D3472" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="E3472" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="3473">
+      <c r="A3473" s="5" t="n">
+        <v>45660</v>
+      </c>
+      <c r="B3473" t="n">
+        <v>33811.97</v>
+      </c>
+      <c r="C3473" t="n">
+        <v>22.66</v>
+      </c>
+      <c r="D3473" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="E3473" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3474">
+      <c r="A3474" s="5" t="n">
+        <v>45663</v>
+      </c>
+      <c r="B3474" t="n">
+        <v>33166.1</v>
+      </c>
+      <c r="C3474" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="D3474" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E3474" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3475">
+      <c r="A3475" s="5" t="n">
+        <v>45664</v>
+      </c>
+      <c r="B3475" t="n">
+        <v>33265.99</v>
+      </c>
+      <c r="C3475" t="n">
+        <v>22.29</v>
+      </c>
+      <c r="D3475" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="E3475" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3476">
+      <c r="A3476" s="5" t="n">
+        <v>45665</v>
+      </c>
+      <c r="B3476" t="n">
+        <v>33195.19</v>
+      </c>
+      <c r="C3476" t="n">
+        <v>22.24</v>
+      </c>
+      <c r="D3476" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E3476" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3477">
+      <c r="A3477" s="5" t="n">
+        <v>45666</v>
+      </c>
+      <c r="B3477" t="n">
+        <v>32931.9</v>
+      </c>
+      <c r="C3477" t="n">
+        <v>22.07</v>
+      </c>
+      <c r="D3477" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="E3477" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="3478">
+      <c r="A3478" s="5" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B3478" t="n">
+        <v>32704.2</v>
+      </c>
+      <c r="C3478" t="n">
+        <v>21.91</v>
+      </c>
+      <c r="D3478" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="E3478" t="n">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="3479">
+      <c r="A3479" s="5" t="n">
+        <v>45670</v>
+      </c>
+      <c r="B3479" t="n">
+        <v>32054.66</v>
+      </c>
+      <c r="C3479" t="n">
+        <v>21.47</v>
+      </c>
+      <c r="D3479" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="E3479" t="n">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="3480">
+      <c r="A3480" s="5" t="n">
+        <v>45671</v>
+      </c>
+      <c r="B3480" t="n">
+        <v>32304.45</v>
+      </c>
+      <c r="C3480" t="n">
+        <v>21.63</v>
+      </c>
+      <c r="D3480" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="E3480" t="n">
+        <v>1.28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>